<commit_message>
Working version: pb_sat; Rsb (expt_rat_8 and 16)
</commit_message>
<xml_diff>
--- a/data/PVT Data_bck.xlsx
+++ b/data/PVT Data_bck.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjdaqua\Python\Projects\HGOR\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjdaqua\Python\Projects\HGOR\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EB8E024-E120-4912-BA2E-93E6B940D60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E76AF0-8ED8-46B3-9E7C-D8A54A53F102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1538,14 +1538,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="E133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1664,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -2552,7 +2551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
@@ -3481,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>15</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>15</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>15</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>6.4085310365158106E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>15</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>6.4908090144355588E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>15</v>
       </c>
@@ -4038,7 +4037,7 @@
         <v>5.3544369541820829E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
@@ -4082,7 +4081,7 @@
         <v>6.0055371052110038E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>15</v>
       </c>
@@ -4125,7 +4124,7 @@
         <v>6.0933996295213034E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>15</v>
       </c>
@@ -4168,7 +4167,7 @@
         <v>5.7037907393253553E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>15</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>6.0055371052110038E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>15</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>5.4414957583540568E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>15</v>
       </c>
@@ -4594,7 +4593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>15</v>
       </c>
@@ -4638,7 +4637,7 @@
         <v>5.3098566869680191E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>15</v>
       </c>
@@ -4682,7 +4681,7 @@
         <v>6.1396776669224863E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>15</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>15</v>
       </c>
@@ -5022,7 +5021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>15</v>
       </c>
@@ -5066,7 +5065,7 @@
         <v>5.5541978627446625E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>15</v>
       </c>
@@ -5279,7 +5278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>15</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:14" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>15</v>
       </c>
@@ -5787,7 +5786,7 @@
         <v>5.4474318725192456E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:14" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>15</v>
       </c>
@@ -8144,134 +8143,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:N156" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="0.05100"/>
-        <filter val="0.0899"/>
-        <filter val="0.09700"/>
-        <filter val="0.11000"/>
-        <filter val="0.12300"/>
-        <filter val="0.12500"/>
-        <filter val="0.1270"/>
-        <filter val="0.12700"/>
-        <filter val="0.1280"/>
-        <filter val="0.13338"/>
-        <filter val="0.1357"/>
-        <filter val="0.13600"/>
-        <filter val="0.1363"/>
-        <filter val="0.13800"/>
-        <filter val="0.1390"/>
-        <filter val="0.1470"/>
-        <filter val="0.14700"/>
-        <filter val="0.15100"/>
-        <filter val="0.15500"/>
-        <filter val="0.1553"/>
-        <filter val="0.1560"/>
-        <filter val="0.16600"/>
-        <filter val="0.16700"/>
-        <filter val="0.1674"/>
-        <filter val="0.16972"/>
-        <filter val="0.17300"/>
-        <filter val="0.174"/>
-        <filter val="0.17400"/>
-        <filter val="0.17436"/>
-        <filter val="0.1760"/>
-        <filter val="0.17600"/>
-        <filter val="0.17700"/>
-        <filter val="0.18006"/>
-        <filter val="0.1830"/>
-        <filter val="0.18400"/>
-        <filter val="0.18500"/>
-        <filter val="0.18600"/>
-        <filter val="0.18800"/>
-        <filter val="0.20000"/>
-        <filter val="0.20800"/>
-        <filter val="0.20900"/>
-        <filter val="0.21000"/>
-        <filter val="0.21029"/>
-        <filter val="0.21100"/>
-        <filter val="0.21300"/>
-        <filter val="0.21500"/>
-        <filter val="0.22300"/>
-        <filter val="0.2286"/>
-        <filter val="0.2320"/>
-        <filter val="0.23500"/>
-        <filter val="0.2352"/>
-        <filter val="0.23800"/>
-        <filter val="0.2420"/>
-        <filter val="0.2425"/>
-        <filter val="0.2450"/>
-        <filter val="0.24900"/>
-        <filter val="0.25400"/>
-        <filter val="0.25700"/>
-        <filter val="0.25900"/>
-        <filter val="0.263"/>
-        <filter val="0.26800"/>
-        <filter val="0.2750"/>
-        <filter val="0.27820"/>
-        <filter val="0.28500"/>
-        <filter val="0.2853"/>
-        <filter val="0.29300"/>
-        <filter val="0.29400"/>
-        <filter val="0.2950"/>
-        <filter val="0.29600"/>
-        <filter val="0.30600"/>
-        <filter val="0.3090"/>
-        <filter val="0.30900"/>
-        <filter val="0.3130"/>
-        <filter val="0.3140"/>
-        <filter val="0.3160"/>
-        <filter val="0.33200"/>
-        <filter val="0.33800"/>
-        <filter val="0.3560"/>
-        <filter val="0.3586"/>
-        <filter val="0.36200"/>
-        <filter val="0.36600"/>
-        <filter val="0.3680"/>
-        <filter val="0.36800"/>
-        <filter val="0.3760"/>
-        <filter val="0.38100"/>
-        <filter val="0.38600"/>
-        <filter val="0.38700"/>
-        <filter val="0.39200"/>
-        <filter val="0.39649"/>
-        <filter val="0.4050"/>
-        <filter val="0.4102"/>
-        <filter val="0.41200"/>
-        <filter val="0.4130"/>
-        <filter val="0.4190"/>
-        <filter val="0.4237"/>
-        <filter val="0.43400"/>
-        <filter val="0.44900"/>
-        <filter val="0.45000"/>
-        <filter val="0.4525"/>
-        <filter val="0.45300"/>
-        <filter val="0.45600"/>
-        <filter val="0.4730"/>
-        <filter val="0.4890"/>
-        <filter val="0.50400"/>
-        <filter val="0.5110"/>
-        <filter val="0.5130"/>
-        <filter val="0.5200"/>
-        <filter val="0.5262"/>
-        <filter val="0.5323"/>
-        <filter val="0.5424"/>
-        <filter val="0.5510"/>
-        <filter val="0.5530"/>
-        <filter val="0.56000"/>
-        <filter val="0.5660"/>
-        <filter val="0.56600"/>
-        <filter val="0.59300"/>
-        <filter val="0.6240"/>
-        <filter val="0.74"/>
-        <filter val="0.9150"/>
-        <filter val="0.9840"/>
-        <filter val="1.1070"/>
-        <filter val="1.17200"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B2:N156" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>